<commit_message>
Actualizar CP y Creacion BD
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Gestión/SGEH-CP.xlsx
+++ b/Desarrollo/SGEH/Gestión/SGEH-CP.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgNI5e5Z4XtsdSlkBYZuvqvTV/ryg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjpPw2pb+b1biTw4Da8MKinpWFgPQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="109">
   <si>
     <t>CRONOGRAMA GENERAL DEL PROYECTO</t>
   </si>
@@ -108,46 +108,43 @@
     <t>Elaboración del Documento de Negocio</t>
   </si>
   <si>
+    <t>León Chavez, Vilca y Mori</t>
+  </si>
+  <si>
+    <t>Hito #1:11/11/2020</t>
+  </si>
+  <si>
+    <t>Analisis y Especificación:</t>
+  </si>
+  <si>
+    <t>Descripción detallada del software</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Entrevista con el cliente</t>
+  </si>
+  <si>
+    <t>León Ortiz</t>
+  </si>
+  <si>
+    <t>Identificación de componentes con que se integra el software</t>
+  </si>
+  <si>
+    <t>Elaboracion de los Requerimientos Funcionales</t>
+  </si>
+  <si>
     <t>León Chavez y Vilca</t>
   </si>
   <si>
-    <t>Hito #1:11/11/2020</t>
-  </si>
-  <si>
-    <t>Analisis y Especificación:</t>
-  </si>
-  <si>
-    <t>Descripción detallada del software</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Todos</t>
-  </si>
-  <si>
-    <t>Entrevista con el cliente</t>
-  </si>
-  <si>
-    <t>León Ortiz</t>
-  </si>
-  <si>
-    <t>Identificación de componentes con que se integra el software</t>
-  </si>
-  <si>
-    <t>Elaboracion de los Requerimientos Funcionales</t>
-  </si>
-  <si>
     <t>Elaboracion de los Requerimientos no Funcionales</t>
   </si>
   <si>
-    <t>Elaboración del documento de análisis</t>
-  </si>
-  <si>
-    <t>Elaboración de diagrama de actividades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">León Ortiz </t>
+    <t>Elaboración de los documentos de Casos de Uso</t>
   </si>
   <si>
     <t>Elaboración de diagramas de casos de uso</t>
@@ -156,9 +153,6 @@
     <t>Elaboración de prototipos</t>
   </si>
   <si>
-    <t>Mori</t>
-  </si>
-  <si>
     <t>Diseño y Arquitectura</t>
   </si>
   <si>
@@ -171,22 +165,22 @@
     <t>Definición de la implementación tecnológica(Hardware,Red)</t>
   </si>
   <si>
-    <t>Asis, Okamoto, Portella</t>
+    <t>Okamoto y Portella</t>
   </si>
   <si>
     <t>Diseño de los componentes de la plataforma(Módulos)</t>
   </si>
   <si>
+    <t>Asis,León Chavez  y Vilca</t>
+  </si>
+  <si>
     <t>Elaboración de documento de diseño</t>
   </si>
   <si>
-    <t>Elaboración de modelamiento de procesos</t>
+    <t>Elaboración de diagrama de clases</t>
   </si>
   <si>
     <t>León Chavez</t>
-  </si>
-  <si>
-    <t>Elaboración de diagrama de clases</t>
   </si>
   <si>
     <t>Elaboracion de Diagramas Entidad Relación</t>
@@ -249,34 +243,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Elaboracion de Store Procedure </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Reservar Evento</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Elaboracion de Store Procedure </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Valoracion de Evento</t>
-    </r>
-  </si>
-  <si>
-    <t>Elaboración de Triggers</t>
-  </si>
-  <si>
-    <t>Elaboración del Backup de Seguridad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elaboración del código del Software </t>
   </si>
   <si>
@@ -295,12 +261,18 @@
     <t>Elaboración de la opción de editar la cuenta</t>
   </si>
   <si>
+    <t>Asis, Okamoto y Mori</t>
+  </si>
+  <si>
     <t>Elaboración de la opción de eliminar cuenta</t>
   </si>
   <si>
     <t>Elaboración de la portada de la web (responsive)</t>
   </si>
   <si>
+    <t>León Chavez, Vilca y Portella</t>
+  </si>
+  <si>
     <t>Elaboración de la sección de agregar servicios</t>
   </si>
   <si>
@@ -316,6 +288,9 @@
     <t>Elaboración de la sección de búsqueda</t>
   </si>
   <si>
+    <t>León Chavez , Vilca y Portella</t>
+  </si>
+  <si>
     <t>Elaboración de la opción de adquirir servicios</t>
   </si>
   <si>
@@ -368,6 +343,9 @@
   </si>
   <si>
     <t>Correccion de posibles errores</t>
+  </si>
+  <si>
+    <t>Asis, Okamoto, Portella</t>
   </si>
   <si>
     <t>Pase a producción:</t>
@@ -847,7 +825,7 @@
     <col customWidth="1" min="3" max="3" width="3.0"/>
     <col customWidth="1" min="4" max="11" width="2.63"/>
     <col customWidth="1" min="12" max="15" width="3.5"/>
-    <col customWidth="1" min="16" max="16" width="21.0"/>
+    <col customWidth="1" min="16" max="16" width="22.63"/>
     <col customWidth="1" min="17" max="26" width="9.38"/>
   </cols>
   <sheetData>
@@ -1152,7 +1130,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="21">
         <v>1.0</v>
@@ -1179,16 +1157,16 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
       <c r="P16" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="21">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17"/>
       <c r="B17" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1206,16 +1184,16 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q17" s="21">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="17"/>
       <c r="B18" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1233,14 +1211,16 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q18" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="17"/>
       <c r="B19" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1258,9 +1238,12 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q19" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T19" s="22"/>
     </row>
     <row r="20">
       <c r="A20" s="17"/>
@@ -1283,14 +1266,15 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q20" s="9"/>
-      <c r="T20" s="22"/>
+        <v>35</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="17"/>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="9"/>
@@ -1298,54 +1282,53 @@
       <c r="E21" s="19"/>
       <c r="F21" s="9"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="19"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="11" t="s">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="Q21" s="9"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="17"/>
-      <c r="B22" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="11"/>
+      <c r="P22" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="Q22" s="9"/>
     </row>
     <row r="23">
-      <c r="B23" s="18" t="s">
-        <v>48</v>
+      <c r="B23" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="18" t="s">
-        <v>34</v>
-      </c>
+      <c r="G23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="19"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -1353,14 +1336,16 @@
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" s="9"/>
+      <c r="P23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1378,7 +1363,7 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="11" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="Q24" s="21">
         <v>1.0</v>
@@ -1392,10 +1377,10 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="19"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -1411,33 +1396,31 @@
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="J26" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q26" s="21">
-        <v>1.0</v>
-      </c>
+      <c r="P26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="9"/>
@@ -1447,22 +1430,24 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="18" t="s">
-        <v>34</v>
+      <c r="J27" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q27" s="9"/>
+      <c r="P27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1480,13 +1465,15 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q28" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="B29" s="19" t="s">
-        <v>56</v>
+      <c r="B29" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1495,22 +1482,18 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="P29" s="11"/>
       <c r="Q29" s="9"/>
     </row>
     <row r="30">
-      <c r="B30" s="19" t="s">
-        <v>57</v>
+      <c r="B30" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1519,62 +1502,68 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
-      <c r="P30" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="P30" s="10"/>
       <c r="Q30" s="9"/>
     </row>
     <row r="31">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
       <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="K31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" s="19"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
-      <c r="P31" s="11"/>
+      <c r="P31" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="Q31" s="9"/>
     </row>
     <row r="32">
-      <c r="B32" s="8" t="s">
-        <v>60</v>
+      <c r="B32" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
       <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="K32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="19"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="9"/>
+      <c r="P32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="B33" s="18" t="s">
-        <v>61</v>
+      <c r="B33" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1584,21 +1573,23 @@
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="18" t="s">
-        <v>34</v>
+      <c r="K33" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
-      <c r="P33" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q33" s="9"/>
+      <c r="P33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1616,9 +1607,11 @@
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
       <c r="P34" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q34" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="19" t="s">
@@ -1640,9 +1633,11 @@
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
       <c r="P35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q35" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="19" t="s">
@@ -1666,180 +1661,181 @@
       <c r="P36" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="Q36" s="9"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="19" t="s">
+      <c r="Q36" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="19"/>
+      <c r="G37" s="9"/>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="11" t="s">
-        <v>55</v>
+      <c r="P37" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38">
-      <c r="B38" s="19" t="s">
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="B38" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L38" s="19"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
-      <c r="P38" s="11" t="s">
-        <v>37</v>
+      <c r="P38" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39">
-      <c r="B39" s="19" t="s">
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="B39" s="26" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="9"/>
-      <c r="K39" s="19" t="s">
+      <c r="K39" s="9"/>
+      <c r="L39" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="19"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
       <c r="P39" s="11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40">
-      <c r="B40" s="19" t="s">
-        <v>70</v>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="B40" s="26" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
       <c r="J40" s="9"/>
-      <c r="K40" s="19" t="s">
+      <c r="K40" s="9"/>
+      <c r="L40" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="19"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
       <c r="P40" s="11" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Q40" s="9"/>
     </row>
-    <row r="41">
-      <c r="B41" s="19" t="s">
-        <v>71</v>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="B41" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
       <c r="J41" s="9"/>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="9"/>
+      <c r="L41" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L41" s="19"/>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="11" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="Q41" s="9"/>
     </row>
-    <row r="42">
-      <c r="A42" s="4"/>
-      <c r="B42" s="19" t="s">
-        <v>72</v>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="B42" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="9"/>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="9"/>
+      <c r="L42" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L42" s="19"/>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="11" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="Q42" s="9"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="18" t="s">
-        <v>73</v>
+      <c r="B43" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="18" t="s">
-        <v>34</v>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
-      <c r="P43" s="20" t="s">
-        <v>35</v>
+      <c r="P43" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="Q43" s="9"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="25" t="s">
-        <v>74</v>
+      <c r="B44" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -1850,20 +1846,20 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="L44" s="18" t="s">
-        <v>34</v>
+      <c r="L44" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
-      <c r="P44" s="20" t="s">
-        <v>35</v>
+      <c r="P44" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="Q44" s="9"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -1881,13 +1877,13 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q45" s="9"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
@@ -1905,13 +1901,13 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
       <c r="P46" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q46" s="9"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -1929,13 +1925,13 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
       <c r="P47" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q47" s="9"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -1953,13 +1949,13 @@
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
       <c r="P48" s="11" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="Q48" s="9"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="26" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -1977,13 +1973,13 @@
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
       <c r="P49" s="11" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="Q49" s="9"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="26" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -2001,13 +1997,13 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
       <c r="P50" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q50" s="9"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="26" t="s">
-        <v>82</v>
+      <c r="B51" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -2018,20 +2014,20 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
-      <c r="L51" s="19" t="s">
-        <v>25</v>
+      <c r="L51" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
-      <c r="P51" s="11" t="s">
-        <v>26</v>
+      <c r="P51" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="26" t="s">
-        <v>83</v>
+      <c r="B52" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -2049,13 +2045,13 @@
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
       <c r="P52" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="26" t="s">
-        <v>84</v>
+      <c r="B53" s="28" t="s">
+        <v>86</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -2073,13 +2069,13 @@
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
       <c r="P53" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="26" t="s">
-        <v>85</v>
+      <c r="B54" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -2097,13 +2093,13 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
       <c r="P54" s="11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="Q54" s="9"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="26" t="s">
-        <v>86</v>
+      <c r="B55" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -2121,13 +2117,13 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="26" t="s">
-        <v>87</v>
+      <c r="B56" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -2145,13 +2141,13 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
       <c r="P56" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q56" s="9"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="27" t="s">
-        <v>88</v>
+      <c r="B57" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2162,20 +2158,20 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
-      <c r="L57" s="18" t="s">
-        <v>34</v>
+      <c r="L57" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
-      <c r="P57" s="20" t="s">
-        <v>35</v>
+      <c r="P57" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="Q57" s="9"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="B58" s="28" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -2193,13 +2189,13 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q58" s="9"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="B59" s="28" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -2217,13 +2213,13 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q59" s="9"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="B60" s="28" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -2241,13 +2237,13 @@
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
       <c r="P60" s="11" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Q60" s="9"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -2265,13 +2261,13 @@
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
       <c r="P61" s="11" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Q61" s="9"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
@@ -2289,13 +2285,13 @@
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
       <c r="P62" s="11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q62" s="9"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="28" t="s">
-        <v>93</v>
+      <c r="B63" s="24" t="s">
+        <v>96</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
@@ -2306,20 +2302,16 @@
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
-      <c r="L63" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
-      <c r="P63" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="P63" s="29"/>
       <c r="Q63" s="9"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="28" t="s">
-        <v>94</v>
+      <c r="B64" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -2330,20 +2322,16 @@
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
-      <c r="L64" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="M64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="19"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
-      <c r="P64" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="P64" s="20"/>
       <c r="Q64" s="9"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="28" t="s">
-        <v>95</v>
+      <c r="B65" s="31" t="s">
+        <v>98</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
@@ -2354,20 +2342,20 @@
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
-      <c r="L65" s="19" t="s">
+      <c r="L65" s="19"/>
+      <c r="M65" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M65" s="9"/>
-      <c r="N65" s="9"/>
+      <c r="N65" s="19"/>
       <c r="O65" s="9"/>
-      <c r="P65" s="11" t="s">
-        <v>26</v>
+      <c r="P65" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q65" s="9"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="28" t="s">
-        <v>96</v>
+      <c r="B66" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
@@ -2378,20 +2366,20 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="19"/>
+      <c r="M66" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
+      <c r="N66" s="19"/>
       <c r="O66" s="9"/>
       <c r="P66" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q66" s="9"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="28" t="s">
-        <v>97</v>
+      <c r="B67" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
@@ -2402,20 +2390,20 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
-      <c r="L67" s="19" t="s">
+      <c r="L67" s="19"/>
+      <c r="M67" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
+      <c r="N67" s="19"/>
       <c r="O67" s="9"/>
       <c r="P67" s="11" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="Q67" s="9"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="28" t="s">
-        <v>98</v>
+      <c r="B68" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -2426,20 +2414,16 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
-      <c r="L68" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="L68" s="9"/>
       <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="N68" s="19"/>
+      <c r="O68" s="19"/>
+      <c r="P68" s="20"/>
       <c r="Q68" s="9"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="24" t="s">
-        <v>99</v>
+      <c r="B69" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
@@ -2451,15 +2435,19 @@
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="29"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O69" s="19"/>
+      <c r="P69" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="Q69" s="9"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="30" t="s">
-        <v>100</v>
+      <c r="B70" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -2471,15 +2459,15 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
-      <c r="M70" s="19"/>
-      <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="19"/>
+      <c r="O70" s="19"/>
       <c r="P70" s="20"/>
       <c r="Q70" s="9"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="31" t="s">
-        <v>101</v>
+      <c r="B71" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -2490,20 +2478,20 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
-      <c r="L71" s="19"/>
-      <c r="M71" s="19" t="s">
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="19"/>
+      <c r="O71" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N71" s="19"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="20" t="s">
-        <v>35</v>
+      <c r="P71" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="Q71" s="9"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="31" t="s">
-        <v>102</v>
+      <c r="B72" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -2514,20 +2502,20 @@
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
-      <c r="L72" s="19"/>
-      <c r="M72" s="19" t="s">
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="19"/>
+      <c r="O72" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N72" s="19"/>
-      <c r="O72" s="9"/>
       <c r="P72" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="Q72" s="9"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="26" t="s">
-        <v>103</v>
+      <c r="B73" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
@@ -2538,148 +2526,30 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
-      <c r="L73" s="19"/>
-      <c r="M73" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N73" s="19"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
       <c r="O73" s="9"/>
-      <c r="P73" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="P73" s="10"/>
       <c r="Q73" s="9"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="19"/>
-      <c r="O74" s="19"/>
-      <c r="P74" s="20"/>
-      <c r="Q74" s="9"/>
+      <c r="P74" s="32"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="O75" s="19"/>
-      <c r="P75" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q75" s="9"/>
+      <c r="P75" s="32"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="19"/>
-      <c r="P76" s="20"/>
-      <c r="Q76" s="9"/>
+      <c r="P76" s="32"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="19"/>
-      <c r="O77" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="P77" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q77" s="9"/>
+      <c r="P77" s="32"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="P78" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q78" s="9"/>
+      <c r="P78" s="32"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="9"/>
-      <c r="N79" s="9"/>
-      <c r="O79" s="9"/>
-      <c r="P79" s="10"/>
-      <c r="Q79" s="9"/>
+      <c r="P79" s="32"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="P80" s="32"/>
@@ -5554,24 +5424,6 @@
     </row>
     <row r="1037" ht="15.75" customHeight="1">
       <c r="P1037" s="32"/>
-    </row>
-    <row r="1038" ht="15.75" customHeight="1">
-      <c r="P1038" s="32"/>
-    </row>
-    <row r="1039" ht="15.75" customHeight="1">
-      <c r="P1039" s="32"/>
-    </row>
-    <row r="1040" ht="15.75" customHeight="1">
-      <c r="P1040" s="32"/>
-    </row>
-    <row r="1041" ht="15.75" customHeight="1">
-      <c r="P1041" s="32"/>
-    </row>
-    <row r="1042" ht="15.75" customHeight="1">
-      <c r="P1042" s="32"/>
-    </row>
-    <row r="1043" ht="15.75" customHeight="1">
-      <c r="P1043" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Actualizar CP y Creacion BD (#16)
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Gestión/SGEH-CP.xlsx
+++ b/Desarrollo/SGEH/Gestión/SGEH-CP.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgNI5e5Z4XtsdSlkBYZuvqvTV/ryg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjpPw2pb+b1biTw4Da8MKinpWFgPQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="109">
   <si>
     <t>CRONOGRAMA GENERAL DEL PROYECTO</t>
   </si>
@@ -108,46 +108,43 @@
     <t>Elaboración del Documento de Negocio</t>
   </si>
   <si>
+    <t>León Chavez, Vilca y Mori</t>
+  </si>
+  <si>
+    <t>Hito #1:11/11/2020</t>
+  </si>
+  <si>
+    <t>Analisis y Especificación:</t>
+  </si>
+  <si>
+    <t>Descripción detallada del software</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Entrevista con el cliente</t>
+  </si>
+  <si>
+    <t>León Ortiz</t>
+  </si>
+  <si>
+    <t>Identificación de componentes con que se integra el software</t>
+  </si>
+  <si>
+    <t>Elaboracion de los Requerimientos Funcionales</t>
+  </si>
+  <si>
     <t>León Chavez y Vilca</t>
   </si>
   <si>
-    <t>Hito #1:11/11/2020</t>
-  </si>
-  <si>
-    <t>Analisis y Especificación:</t>
-  </si>
-  <si>
-    <t>Descripción detallada del software</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Todos</t>
-  </si>
-  <si>
-    <t>Entrevista con el cliente</t>
-  </si>
-  <si>
-    <t>León Ortiz</t>
-  </si>
-  <si>
-    <t>Identificación de componentes con que se integra el software</t>
-  </si>
-  <si>
-    <t>Elaboracion de los Requerimientos Funcionales</t>
-  </si>
-  <si>
     <t>Elaboracion de los Requerimientos no Funcionales</t>
   </si>
   <si>
-    <t>Elaboración del documento de análisis</t>
-  </si>
-  <si>
-    <t>Elaboración de diagrama de actividades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">León Ortiz </t>
+    <t>Elaboración de los documentos de Casos de Uso</t>
   </si>
   <si>
     <t>Elaboración de diagramas de casos de uso</t>
@@ -156,9 +153,6 @@
     <t>Elaboración de prototipos</t>
   </si>
   <si>
-    <t>Mori</t>
-  </si>
-  <si>
     <t>Diseño y Arquitectura</t>
   </si>
   <si>
@@ -171,22 +165,22 @@
     <t>Definición de la implementación tecnológica(Hardware,Red)</t>
   </si>
   <si>
-    <t>Asis, Okamoto, Portella</t>
+    <t>Okamoto y Portella</t>
   </si>
   <si>
     <t>Diseño de los componentes de la plataforma(Módulos)</t>
   </si>
   <si>
+    <t>Asis,León Chavez  y Vilca</t>
+  </si>
+  <si>
     <t>Elaboración de documento de diseño</t>
   </si>
   <si>
-    <t>Elaboración de modelamiento de procesos</t>
+    <t>Elaboración de diagrama de clases</t>
   </si>
   <si>
     <t>León Chavez</t>
-  </si>
-  <si>
-    <t>Elaboración de diagrama de clases</t>
   </si>
   <si>
     <t>Elaboracion de Diagramas Entidad Relación</t>
@@ -249,34 +243,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Elaboracion de Store Procedure </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Reservar Evento</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Elaboracion de Store Procedure </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Valoracion de Evento</t>
-    </r>
-  </si>
-  <si>
-    <t>Elaboración de Triggers</t>
-  </si>
-  <si>
-    <t>Elaboración del Backup de Seguridad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elaboración del código del Software </t>
   </si>
   <si>
@@ -295,12 +261,18 @@
     <t>Elaboración de la opción de editar la cuenta</t>
   </si>
   <si>
+    <t>Asis, Okamoto y Mori</t>
+  </si>
+  <si>
     <t>Elaboración de la opción de eliminar cuenta</t>
   </si>
   <si>
     <t>Elaboración de la portada de la web (responsive)</t>
   </si>
   <si>
+    <t>León Chavez, Vilca y Portella</t>
+  </si>
+  <si>
     <t>Elaboración de la sección de agregar servicios</t>
   </si>
   <si>
@@ -316,6 +288,9 @@
     <t>Elaboración de la sección de búsqueda</t>
   </si>
   <si>
+    <t>León Chavez , Vilca y Portella</t>
+  </si>
+  <si>
     <t>Elaboración de la opción de adquirir servicios</t>
   </si>
   <si>
@@ -368,6 +343,9 @@
   </si>
   <si>
     <t>Correccion de posibles errores</t>
+  </si>
+  <si>
+    <t>Asis, Okamoto, Portella</t>
   </si>
   <si>
     <t>Pase a producción:</t>
@@ -847,7 +825,7 @@
     <col customWidth="1" min="3" max="3" width="3.0"/>
     <col customWidth="1" min="4" max="11" width="2.63"/>
     <col customWidth="1" min="12" max="15" width="3.5"/>
-    <col customWidth="1" min="16" max="16" width="21.0"/>
+    <col customWidth="1" min="16" max="16" width="22.63"/>
     <col customWidth="1" min="17" max="26" width="9.38"/>
   </cols>
   <sheetData>
@@ -1152,7 +1130,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="21">
         <v>1.0</v>
@@ -1179,16 +1157,16 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
       <c r="P16" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="21">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17"/>
       <c r="B17" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1206,16 +1184,16 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q17" s="21">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="17"/>
       <c r="B18" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1233,14 +1211,16 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q18" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="17"/>
       <c r="B19" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1258,9 +1238,12 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q19" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T19" s="22"/>
     </row>
     <row r="20">
       <c r="A20" s="17"/>
@@ -1283,14 +1266,15 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q20" s="9"/>
-      <c r="T20" s="22"/>
+        <v>35</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="17"/>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="9"/>
@@ -1298,54 +1282,53 @@
       <c r="E21" s="19"/>
       <c r="F21" s="9"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="19"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="11" t="s">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="Q21" s="9"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="17"/>
-      <c r="B22" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="11"/>
+      <c r="P22" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="Q22" s="9"/>
     </row>
     <row r="23">
-      <c r="B23" s="18" t="s">
-        <v>48</v>
+      <c r="B23" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="18" t="s">
-        <v>34</v>
-      </c>
+      <c r="G23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="19"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -1353,14 +1336,16 @@
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" s="9"/>
+      <c r="P23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1378,7 +1363,7 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="11" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="Q24" s="21">
         <v>1.0</v>
@@ -1392,10 +1377,10 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="19"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -1411,33 +1396,31 @@
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="J26" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q26" s="21">
-        <v>1.0</v>
-      </c>
+      <c r="P26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="9"/>
@@ -1447,22 +1430,24 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="18" t="s">
-        <v>34</v>
+      <c r="J27" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q27" s="9"/>
+      <c r="P27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1480,13 +1465,15 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q28" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="B29" s="19" t="s">
-        <v>56</v>
+      <c r="B29" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1495,22 +1482,18 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="P29" s="11"/>
       <c r="Q29" s="9"/>
     </row>
     <row r="30">
-      <c r="B30" s="19" t="s">
-        <v>57</v>
+      <c r="B30" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1519,62 +1502,68 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
-      <c r="P30" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="P30" s="10"/>
       <c r="Q30" s="9"/>
     </row>
     <row r="31">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
       <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="K31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" s="19"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
-      <c r="P31" s="11"/>
+      <c r="P31" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="Q31" s="9"/>
     </row>
     <row r="32">
-      <c r="B32" s="8" t="s">
-        <v>60</v>
+      <c r="B32" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
       <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="K32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="19"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="9"/>
+      <c r="P32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="B33" s="18" t="s">
-        <v>61</v>
+      <c r="B33" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1584,21 +1573,23 @@
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="18" t="s">
-        <v>34</v>
+      <c r="K33" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
-      <c r="P33" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q33" s="9"/>
+      <c r="P33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1616,9 +1607,11 @@
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
       <c r="P34" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q34" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="19" t="s">
@@ -1640,9 +1633,11 @@
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
       <c r="P35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q35" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="19" t="s">
@@ -1666,180 +1661,181 @@
       <c r="P36" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="Q36" s="9"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="19" t="s">
+      <c r="Q36" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="19"/>
+      <c r="G37" s="9"/>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="11" t="s">
-        <v>55</v>
+      <c r="P37" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38">
-      <c r="B38" s="19" t="s">
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="B38" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L38" s="19"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
-      <c r="P38" s="11" t="s">
-        <v>37</v>
+      <c r="P38" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39">
-      <c r="B39" s="19" t="s">
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="B39" s="26" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="9"/>
-      <c r="K39" s="19" t="s">
+      <c r="K39" s="9"/>
+      <c r="L39" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="19"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
       <c r="P39" s="11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40">
-      <c r="B40" s="19" t="s">
-        <v>70</v>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="B40" s="26" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
       <c r="J40" s="9"/>
-      <c r="K40" s="19" t="s">
+      <c r="K40" s="9"/>
+      <c r="L40" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="19"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
       <c r="P40" s="11" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Q40" s="9"/>
     </row>
-    <row r="41">
-      <c r="B41" s="19" t="s">
-        <v>71</v>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="B41" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
       <c r="J41" s="9"/>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="9"/>
+      <c r="L41" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L41" s="19"/>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="11" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="Q41" s="9"/>
     </row>
-    <row r="42">
-      <c r="A42" s="4"/>
-      <c r="B42" s="19" t="s">
-        <v>72</v>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="B42" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="9"/>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="9"/>
+      <c r="L42" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L42" s="19"/>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="11" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="Q42" s="9"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="18" t="s">
-        <v>73</v>
+      <c r="B43" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="18" t="s">
-        <v>34</v>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
-      <c r="P43" s="20" t="s">
-        <v>35</v>
+      <c r="P43" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="Q43" s="9"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="25" t="s">
-        <v>74</v>
+      <c r="B44" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -1850,20 +1846,20 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="L44" s="18" t="s">
-        <v>34</v>
+      <c r="L44" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
-      <c r="P44" s="20" t="s">
-        <v>35</v>
+      <c r="P44" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="Q44" s="9"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -1881,13 +1877,13 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q45" s="9"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
@@ -1905,13 +1901,13 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
       <c r="P46" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q46" s="9"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -1929,13 +1925,13 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
       <c r="P47" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q47" s="9"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -1953,13 +1949,13 @@
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
       <c r="P48" s="11" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="Q48" s="9"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="26" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -1977,13 +1973,13 @@
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
       <c r="P49" s="11" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="Q49" s="9"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="26" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -2001,13 +1997,13 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
       <c r="P50" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q50" s="9"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="26" t="s">
-        <v>82</v>
+      <c r="B51" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -2018,20 +2014,20 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
-      <c r="L51" s="19" t="s">
-        <v>25</v>
+      <c r="L51" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
-      <c r="P51" s="11" t="s">
-        <v>26</v>
+      <c r="P51" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="26" t="s">
-        <v>83</v>
+      <c r="B52" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -2049,13 +2045,13 @@
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
       <c r="P52" s="11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="26" t="s">
-        <v>84</v>
+      <c r="B53" s="28" t="s">
+        <v>86</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -2073,13 +2069,13 @@
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
       <c r="P53" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="26" t="s">
-        <v>85</v>
+      <c r="B54" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -2097,13 +2093,13 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
       <c r="P54" s="11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="Q54" s="9"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="26" t="s">
-        <v>86</v>
+      <c r="B55" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -2121,13 +2117,13 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="26" t="s">
-        <v>87</v>
+      <c r="B56" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -2145,13 +2141,13 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
       <c r="P56" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q56" s="9"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="27" t="s">
-        <v>88</v>
+      <c r="B57" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2162,20 +2158,20 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
-      <c r="L57" s="18" t="s">
-        <v>34</v>
+      <c r="L57" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
-      <c r="P57" s="20" t="s">
-        <v>35</v>
+      <c r="P57" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="Q57" s="9"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="B58" s="28" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -2193,13 +2189,13 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q58" s="9"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="B59" s="28" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -2217,13 +2213,13 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="11" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="Q59" s="9"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="B60" s="28" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -2241,13 +2237,13 @@
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
       <c r="P60" s="11" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Q60" s="9"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -2265,13 +2261,13 @@
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
       <c r="P61" s="11" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Q61" s="9"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
@@ -2289,13 +2285,13 @@
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
       <c r="P62" s="11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q62" s="9"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="28" t="s">
-        <v>93</v>
+      <c r="B63" s="24" t="s">
+        <v>96</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
@@ -2306,20 +2302,16 @@
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
-      <c r="L63" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
-      <c r="P63" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="P63" s="29"/>
       <c r="Q63" s="9"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="28" t="s">
-        <v>94</v>
+      <c r="B64" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -2330,20 +2322,16 @@
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
-      <c r="L64" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="M64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="19"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
-      <c r="P64" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="P64" s="20"/>
       <c r="Q64" s="9"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="28" t="s">
-        <v>95</v>
+      <c r="B65" s="31" t="s">
+        <v>98</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
@@ -2354,20 +2342,20 @@
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
-      <c r="L65" s="19" t="s">
+      <c r="L65" s="19"/>
+      <c r="M65" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M65" s="9"/>
-      <c r="N65" s="9"/>
+      <c r="N65" s="19"/>
       <c r="O65" s="9"/>
-      <c r="P65" s="11" t="s">
-        <v>26</v>
+      <c r="P65" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="Q65" s="9"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="28" t="s">
-        <v>96</v>
+      <c r="B66" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
@@ -2378,20 +2366,20 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="19"/>
+      <c r="M66" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
+      <c r="N66" s="19"/>
       <c r="O66" s="9"/>
       <c r="P66" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q66" s="9"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="28" t="s">
-        <v>97</v>
+      <c r="B67" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
@@ -2402,20 +2390,20 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
-      <c r="L67" s="19" t="s">
+      <c r="L67" s="19"/>
+      <c r="M67" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
+      <c r="N67" s="19"/>
       <c r="O67" s="9"/>
       <c r="P67" s="11" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="Q67" s="9"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="28" t="s">
-        <v>98</v>
+      <c r="B68" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -2426,20 +2414,16 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
-      <c r="L68" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="L68" s="9"/>
       <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="N68" s="19"/>
+      <c r="O68" s="19"/>
+      <c r="P68" s="20"/>
       <c r="Q68" s="9"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="24" t="s">
-        <v>99</v>
+      <c r="B69" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
@@ -2451,15 +2435,19 @@
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="29"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O69" s="19"/>
+      <c r="P69" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="Q69" s="9"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="30" t="s">
-        <v>100</v>
+      <c r="B70" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -2471,15 +2459,15 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
-      <c r="M70" s="19"/>
-      <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="19"/>
+      <c r="O70" s="19"/>
       <c r="P70" s="20"/>
       <c r="Q70" s="9"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="31" t="s">
-        <v>101</v>
+      <c r="B71" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -2490,20 +2478,20 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
-      <c r="L71" s="19"/>
-      <c r="M71" s="19" t="s">
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="19"/>
+      <c r="O71" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N71" s="19"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="20" t="s">
-        <v>35</v>
+      <c r="P71" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="Q71" s="9"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="31" t="s">
-        <v>102</v>
+      <c r="B72" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -2514,20 +2502,20 @@
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
-      <c r="L72" s="19"/>
-      <c r="M72" s="19" t="s">
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="19"/>
+      <c r="O72" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N72" s="19"/>
-      <c r="O72" s="9"/>
       <c r="P72" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="Q72" s="9"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="26" t="s">
-        <v>103</v>
+      <c r="B73" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
@@ -2538,148 +2526,30 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
-      <c r="L73" s="19"/>
-      <c r="M73" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N73" s="19"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
       <c r="O73" s="9"/>
-      <c r="P73" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="P73" s="10"/>
       <c r="Q73" s="9"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="19"/>
-      <c r="O74" s="19"/>
-      <c r="P74" s="20"/>
-      <c r="Q74" s="9"/>
+      <c r="P74" s="32"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="O75" s="19"/>
-      <c r="P75" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q75" s="9"/>
+      <c r="P75" s="32"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="19"/>
-      <c r="P76" s="20"/>
-      <c r="Q76" s="9"/>
+      <c r="P76" s="32"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="19"/>
-      <c r="O77" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="P77" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q77" s="9"/>
+      <c r="P77" s="32"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="P78" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q78" s="9"/>
+      <c r="P78" s="32"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="9"/>
-      <c r="N79" s="9"/>
-      <c r="O79" s="9"/>
-      <c r="P79" s="10"/>
-      <c r="Q79" s="9"/>
+      <c r="P79" s="32"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="P80" s="32"/>
@@ -5554,24 +5424,6 @@
     </row>
     <row r="1037" ht="15.75" customHeight="1">
       <c r="P1037" s="32"/>
-    </row>
-    <row r="1038" ht="15.75" customHeight="1">
-      <c r="P1038" s="32"/>
-    </row>
-    <row r="1039" ht="15.75" customHeight="1">
-      <c r="P1039" s="32"/>
-    </row>
-    <row r="1040" ht="15.75" customHeight="1">
-      <c r="P1040" s="32"/>
-    </row>
-    <row r="1041" ht="15.75" customHeight="1">
-      <c r="P1041" s="32"/>
-    </row>
-    <row r="1042" ht="15.75" customHeight="1">
-      <c r="P1042" s="32"/>
-    </row>
-    <row r="1043" ht="15.75" customHeight="1">
-      <c r="P1043" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>